<commit_message>
Calculated total sal and annual sal of the employees
</commit_message>
<xml_diff>
--- a/Employee Data.xlsx
+++ b/Employee Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Power BI\Sample data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3264b996da2e285a/Desktop/Demo project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A46022-CD50-46E5-99E4-ACCE83EF4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{14A46022-CD50-46E5-99E4-ACCE83EF4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C14FF38-1B6D-4348-A0D6-37234CB2FA0D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A9EA8D1C-46E6-41F3-8DDB-531692A1F2CD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>EmpID</t>
   </si>
@@ -230,12 +230,18 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Annual sal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,7 +288,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{310E3032-C5C4-4827-AA3C-53E56340FF25}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -593,7 +601,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B1E619-45F4-4940-81BA-9E84F12D59D0}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -629,6 +639,12 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -655,6 +671,14 @@
       <c r="H2">
         <v>600</v>
       </c>
+      <c r="I2">
+        <f>E2+H2</f>
+        <v>20600</v>
+      </c>
+      <c r="J2">
+        <f>I2*12</f>
+        <v>247200</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -681,6 +705,14 @@
       <c r="H3">
         <v>700</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I22" si="0">E3+H3</f>
+        <v>10700</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J22" si="1">I3*12</f>
+        <v>128400</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -707,6 +739,14 @@
       <c r="H4">
         <v>800</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>18800</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>225600</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -733,6 +773,14 @@
       <c r="H5">
         <v>600</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>18600</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>223200</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -760,6 +808,14 @@
       <c r="H6">
         <v>600</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>18600</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>223200</v>
+      </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,6 +843,14 @@
       <c r="H7">
         <v>500</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>10500</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>126000</v>
+      </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -814,6 +878,14 @@
       <c r="H8">
         <v>300</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>15300</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>183600</v>
+      </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -841,6 +913,14 @@
       <c r="H9">
         <v>400</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>15400</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>184800</v>
+      </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,6 +948,14 @@
       <c r="H10">
         <v>300</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>63600</v>
+      </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -895,6 +983,14 @@
       <c r="H11">
         <v>300</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>63600</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -922,6 +1018,14 @@
       <c r="H12">
         <v>300</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>12300</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>147600</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -949,6 +1053,14 @@
       <c r="H13">
         <v>600</v>
       </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>12600</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>151200</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -976,6 +1088,14 @@
       <c r="H14">
         <v>600</v>
       </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>13600</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>163200</v>
+      </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1003,6 +1123,14 @@
       <c r="H15">
         <v>600</v>
       </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>259200</v>
+      </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1030,6 +1158,14 @@
       <c r="H16">
         <v>600</v>
       </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>259200</v>
+      </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1057,6 +1193,14 @@
       <c r="H17">
         <v>1000</v>
       </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>56000</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>672000</v>
+      </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1084,6 +1228,14 @@
       <c r="H18">
         <v>800</v>
       </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>40800</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>489600</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1110,6 +1262,14 @@
       <c r="H19">
         <v>800</v>
       </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>25800</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>309600</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1136,6 +1296,14 @@
       <c r="H20">
         <v>800</v>
       </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>27800</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>333600</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1162,6 +1330,14 @@
       <c r="H21">
         <v>400</v>
       </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>23400</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>280800</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1187,6 +1363,14 @@
       </c>
       <c r="H22">
         <v>800</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>25800</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>309600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text added in main.txt file
</commit_message>
<xml_diff>
--- a/Employee Data.xlsx
+++ b/Employee Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3264b996da2e285a/Desktop/Demo project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{14A46022-CD50-46E5-99E4-ACCE83EF4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C14FF38-1B6D-4348-A0D6-37234CB2FA0D}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{14A46022-CD50-46E5-99E4-ACCE83EF4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E52020C2-6E5D-4008-9CED-F9E54A272B77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A9EA8D1C-46E6-41F3-8DDB-531692A1F2CD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>EmpID</t>
   </si>
@@ -236,13 +236,25 @@
   </si>
   <si>
     <t>Annual sal</t>
+  </si>
+  <si>
+    <t>Aparna</t>
+  </si>
+  <si>
+    <t>Viswanath</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>Gupta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +268,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,10 +284,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -277,12 +322,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,778 +646,851 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B1E619-45F4-4940-81BA-9E84F12D59D0}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="156" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1002</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>20000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>600</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <f>E2+H2</f>
         <v>20600</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <f>I2*12</f>
         <v>247200</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1003</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>10000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>700</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I22" si="0">E3+H3</f>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I23" si="0">E3+H3</f>
         <v>10700</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J22" si="1">I3*12</f>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J24" si="1">I3*12</f>
         <v>128400</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>1004</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>18000</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>800</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>18800</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f t="shared" si="1"/>
         <v>225600</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1005</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>18000</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>600</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>18600</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <f t="shared" si="1"/>
         <v>223200</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>1006</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>18000</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>600</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>18600</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <f t="shared" si="1"/>
         <v>223200</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>1007</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>10000</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>500</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>10500</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <f t="shared" si="1"/>
         <v>126000</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>1008</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>15000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>300</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>15300</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <f t="shared" si="1"/>
         <v>183600</v>
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>1009</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>15000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>400</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>15400</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
         <v>184800</v>
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>1009</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>5000</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>300</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>5300</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="2">
         <f t="shared" si="1"/>
         <v>63600</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>1010</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>5000</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>300</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <f t="shared" si="0"/>
         <v>5300</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <f t="shared" si="1"/>
         <v>63600</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1002</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1011</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>12000</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>1</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>300</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>12300</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="2">
         <f t="shared" si="1"/>
         <v>147600</v>
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1002</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1012</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>12000</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>3</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>600</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <f t="shared" si="0"/>
         <v>12600</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <f t="shared" si="1"/>
         <v>151200</v>
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1002</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1013</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>13000</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>3</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>600</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <f t="shared" si="0"/>
         <v>13600</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="2">
         <f t="shared" si="1"/>
         <v>163200</v>
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1002</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1014</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>21000</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>4</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>600</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>21600</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="2">
         <f t="shared" si="1"/>
         <v>259200</v>
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1002</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1015</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>21000</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>4</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>600</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <f t="shared" si="0"/>
         <v>21600</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <f t="shared" si="1"/>
         <v>259200</v>
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1002</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>1016</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>55000</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>9</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <v>1000</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <f t="shared" si="0"/>
         <v>56000</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="2">
         <f t="shared" si="1"/>
         <v>672000</v>
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1002</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>1017</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>40000</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>7</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>800</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <f t="shared" si="0"/>
         <v>40800</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <f t="shared" si="1"/>
         <v>489600</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1002</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>1018</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>25000</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>7</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>800</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <f t="shared" si="0"/>
         <v>25800</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="2">
         <f t="shared" si="1"/>
         <v>309600</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1002</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>1019</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>27000</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>7</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>800</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="2">
         <f t="shared" si="0"/>
         <v>27800</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <f t="shared" si="1"/>
         <v>333600</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1002</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>1020</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>23000</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>3</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <v>400</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <f t="shared" si="0"/>
         <v>23400</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <f t="shared" si="1"/>
         <v>280800</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1002</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>1021</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>25000</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>6</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>800</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <f t="shared" si="0"/>
         <v>25800</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <f t="shared" si="1"/>
         <v>309600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>1022</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="4">
+        <v>31000</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>900</v>
+      </c>
+      <c r="I23" s="4">
+        <f>E23+H23</f>
+        <v>31900</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="1"/>
+        <v>382800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="4">
+        <v>28000</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3</v>
+      </c>
+      <c r="H24" s="4">
+        <v>500</v>
+      </c>
+      <c r="I24" s="4">
+        <f>E24+H24</f>
+        <v>28500</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="1"/>
+        <v>342000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>